<commit_message>
Docs: se egrega propuesta v3
</commit_message>
<xml_diff>
--- a/02-Diseño/01-UML/01-Caso_de_Uso_y_Caso_de_Uso_Extendido/Caso_de_uso_v2/Pendiente_por_caso_uso_extendido_y_MKBS.xlsx
+++ b/02-Diseño/01-UML/01-Caso_de_Uso_y_Caso_de_Uso_Extendido/Caso_de_uso_v2/Pendiente_por_caso_uso_extendido_y_MKBS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Rol</t>
   </si>
@@ -48,6 +48,30 @@
   </si>
   <si>
     <t>Consulta productos</t>
+  </si>
+  <si>
+    <t>Consulta clientes</t>
+  </si>
+  <si>
+    <t>Se modifica de crear a crud</t>
+  </si>
+  <si>
+    <t>Bodega</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>CRUD usuario</t>
+  </si>
+  <si>
+    <t>Habilita cuenta</t>
+  </si>
+  <si>
+    <t>Clasifica usuario</t>
+  </si>
+  <si>
+    <t>Clasifica producto</t>
   </si>
 </sst>
 </file>
@@ -365,13 +389,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -428,6 +455,72 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>